<commit_message>
Update accommodations files with spec values only
The files were updated to contain only values that are listed
in the Test Results Transmission specification.
</commit_message>
<xml_diff>
--- a/irp-package/IRPStudentsDesignatedSupportsAndAccommodations.xlsx
+++ b/irp-package/IRPStudentsDesignatedSupportsAndAccommodations.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Espinosa/Development/SmarterBalanced/ireadinesspackage/irp-webapp/src/main/resources/irp-package/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Espinosa/Development/SmarterBalanced/irp-package/irp-package/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9400" yWindow="6240" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="DESIGNATEDSUPPORTSANDACCOMMODAT" sheetId="1" r:id="rId1"/>
@@ -68,16 +68,16 @@
     <t>IRP119990001</t>
   </si>
   <si>
-    <t>|TDS_Masking0|NEDS_SC_Items|NEA_AR|NEA_RA_Stimuli</t>
-  </si>
-  <si>
-    <t>|TDS_CCInvert|TDS_Masking1|TDS_TTS_Stim|NEDS_Mag|NEDS_RA_Items|NEDS_SC_Items|NEDS_SS|TDS_PoD_Item|TDS_SLM1</t>
-  </si>
-  <si>
-    <t>|TDS_WL_ESNGlossary&amp;TDS_WL_Glossary|TDS_Masking0</t>
-  </si>
-  <si>
-    <t>|TDS_SLM0|TDS_CC0|TDS_Masking0|NEDS_CC</t>
+    <t>|TDS_CC0|TDS_Masking0|NEDS_CC</t>
+  </si>
+  <si>
+    <t>|TDS_Masking0|NEDS_SC_Items</t>
+  </si>
+  <si>
+    <t>|TDS_CCInvert|TDS_Masking1|TDS_TTS_Stim|NEDS_Mag|NEDS_RA_Items|NEDS_SC_Items|NEDS_SS</t>
+  </si>
+  <si>
+    <t>|TDS_Masking1</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -463,7 +463,7 @@
     <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="98.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -531,7 +531,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3"/>
       <c r="F3"/>
@@ -558,7 +558,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4"/>
       <c r="F4"/>
@@ -585,7 +585,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
@@ -612,7 +612,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>

</xml_diff>